<commit_message>
add car and walk's attribute for transportation role
</commit_message>
<xml_diff>
--- a/rule_test.xlsx
+++ b/rule_test.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3780" yWindow="1020" windowWidth="29720" windowHeight="14920" tabRatio="500"/>
+    <workbookView xWindow="1360" yWindow="2060" windowWidth="29720" windowHeight="14920" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="45">
   <si>
     <t>ID</t>
   </si>
@@ -157,6 +157,12 @@
   </si>
   <si>
     <t>location_to_be_fired</t>
+  </si>
+  <si>
+    <t>car</t>
+  </si>
+  <si>
+    <t>walk</t>
   </si>
 </sst>
 </file>
@@ -212,8 +218,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -224,9 +236,15 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -502,15 +520,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U41"/>
+  <dimension ref="A1:AE57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U1" sqref="U1"/>
+    <sheetView tabSelected="1" topLeftCell="Q31" workbookViewId="0">
+      <selection activeCell="AE57" sqref="AE57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="20" max="20" width="21.5" customWidth="1"/>
+    <col min="21" max="21" width="29.5" customWidth="1"/>
+    <col min="22" max="22" width="27.33203125" customWidth="1"/>
+    <col min="23" max="23" width="19.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -539,219 +563,249 @@
         <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="S1" t="s">
+      <c r="AC1" t="s">
         <v>37</v>
       </c>
-      <c r="T1" t="s">
+      <c r="AD1" t="s">
         <v>38</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-      <c r="O2">
-        <v>1</v>
-      </c>
-      <c r="U2" t="s">
+      <c r="T2">
+        <v>1</v>
+      </c>
+      <c r="Y2">
+        <v>1</v>
+      </c>
+      <c r="AE2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
-      <c r="O3">
+      <c r="Y3">
         <v>-1</v>
       </c>
-      <c r="U3" t="s">
+      <c r="AE3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
-      <c r="O4">
+      <c r="Y4">
         <v>-2</v>
       </c>
-      <c r="U4" t="s">
+      <c r="AE4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
-      <c r="J5">
-        <v>1</v>
-      </c>
-      <c r="O5">
-        <v>1</v>
-      </c>
-      <c r="U5" t="s">
+      <c r="T5">
+        <v>1</v>
+      </c>
+      <c r="Y5">
+        <v>1</v>
+      </c>
+      <c r="AE5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
-      <c r="O6">
+      <c r="Y6">
         <v>-1</v>
       </c>
-      <c r="U6" t="s">
+      <c r="AE6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="D7">
         <v>2</v>
       </c>
-      <c r="O7">
+      <c r="Y7">
         <v>-2</v>
       </c>
-      <c r="U7" t="s">
+      <c r="AE7" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
-      <c r="K8">
+      <c r="U8">
         <v>-2</v>
       </c>
-      <c r="U8" t="s">
+      <c r="AE8" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
-      <c r="K9">
+      <c r="U9">
         <v>-1</v>
       </c>
-      <c r="U9" t="s">
+      <c r="AE9" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="C10">
         <v>2</v>
       </c>
-      <c r="K10">
-        <v>1</v>
-      </c>
-      <c r="U10" t="s">
+      <c r="U10">
+        <v>1</v>
+      </c>
+      <c r="AE10" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="E11">
         <v>0</v>
       </c>
-      <c r="U11" t="s">
+      <c r="AE11" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="E12">
         <v>1</v>
       </c>
-      <c r="U12" t="s">
+      <c r="AE12" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="F13">
         <v>0</v>
       </c>
-      <c r="U13" t="s">
+      <c r="AE13" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="F14">
         <v>1</v>
       </c>
-      <c r="U14" t="s">
+      <c r="AE14" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -764,14 +818,14 @@
       <c r="I15">
         <v>0</v>
       </c>
-      <c r="S15">
-        <v>1</v>
-      </c>
-      <c r="U15" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="AC15">
+        <v>1</v>
+      </c>
+      <c r="AE15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -784,14 +838,14 @@
       <c r="I16">
         <v>1</v>
       </c>
-      <c r="S16">
-        <v>1</v>
-      </c>
-      <c r="U16" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="AC16">
+        <v>1</v>
+      </c>
+      <c r="AE16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -804,14 +858,14 @@
       <c r="I17">
         <v>2</v>
       </c>
-      <c r="T17">
-        <v>1</v>
-      </c>
-      <c r="U17" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="AD17">
+        <v>1</v>
+      </c>
+      <c r="AE17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -824,14 +878,14 @@
       <c r="I18">
         <v>0</v>
       </c>
-      <c r="S18">
-        <v>1</v>
-      </c>
-      <c r="U18" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="AC18">
+        <v>1</v>
+      </c>
+      <c r="AE18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -844,17 +898,17 @@
       <c r="I19">
         <v>1</v>
       </c>
-      <c r="S19">
-        <v>1</v>
-      </c>
-      <c r="T19">
-        <v>1</v>
-      </c>
-      <c r="U19" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="AC19">
+        <v>1</v>
+      </c>
+      <c r="AD19">
+        <v>1</v>
+      </c>
+      <c r="AE19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -867,14 +921,14 @@
       <c r="I20">
         <v>2</v>
       </c>
-      <c r="T20">
-        <v>1</v>
-      </c>
-      <c r="U20" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="AD20">
+        <v>1</v>
+      </c>
+      <c r="AE20" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -887,14 +941,14 @@
       <c r="I21">
         <v>0</v>
       </c>
-      <c r="S21">
-        <v>1</v>
-      </c>
-      <c r="U21" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="AC21">
+        <v>1</v>
+      </c>
+      <c r="AE21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -907,14 +961,14 @@
       <c r="I22">
         <v>1</v>
       </c>
-      <c r="S22">
-        <v>1</v>
-      </c>
-      <c r="U22" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="AC22">
+        <v>1</v>
+      </c>
+      <c r="AE22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -927,14 +981,14 @@
       <c r="I23">
         <v>2</v>
       </c>
-      <c r="S23">
-        <v>1</v>
-      </c>
-      <c r="U23" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="AC23">
+        <v>1</v>
+      </c>
+      <c r="AE23" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -947,14 +1001,14 @@
       <c r="I24">
         <v>0</v>
       </c>
-      <c r="T24" s="1">
-        <v>1</v>
-      </c>
-      <c r="U24" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="AD24" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE24" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -967,14 +1021,14 @@
       <c r="I25">
         <v>1</v>
       </c>
-      <c r="T25" s="1">
-        <v>1</v>
-      </c>
-      <c r="U25" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="AD25" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE25" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -987,14 +1041,14 @@
       <c r="I26">
         <v>2</v>
       </c>
-      <c r="T26" s="1">
-        <v>1</v>
-      </c>
-      <c r="U26" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="AD26" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE26" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1007,14 +1061,14 @@
       <c r="I27">
         <v>0</v>
       </c>
-      <c r="T27" s="1">
-        <v>1</v>
-      </c>
-      <c r="U27" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="AD27" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE27" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="28" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1027,14 +1081,14 @@
       <c r="I28">
         <v>1</v>
       </c>
-      <c r="T28" s="1">
-        <v>1</v>
-      </c>
-      <c r="U28" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="AD28" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE28" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1047,14 +1101,14 @@
       <c r="I29">
         <v>2</v>
       </c>
-      <c r="T29" s="1">
-        <v>1</v>
-      </c>
-      <c r="U29" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="AD29" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE29" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="30" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1067,14 +1121,14 @@
       <c r="I30">
         <v>0</v>
       </c>
-      <c r="T30" s="1">
-        <v>1</v>
-      </c>
-      <c r="U30" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="AD30" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE30" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="31" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1087,14 +1141,14 @@
       <c r="I31">
         <v>1</v>
       </c>
-      <c r="T31" s="1">
-        <v>1</v>
-      </c>
-      <c r="U31" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="AD31" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE31" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="32" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1107,14 +1161,14 @@
       <c r="I32">
         <v>2</v>
       </c>
-      <c r="T32" s="1">
-        <v>1</v>
-      </c>
-      <c r="U32" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="AD32" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE32" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="33" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1127,14 +1181,14 @@
       <c r="I33">
         <v>0</v>
       </c>
-      <c r="T33">
-        <v>1</v>
-      </c>
-      <c r="U33" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="AD33">
+        <v>1</v>
+      </c>
+      <c r="AE33" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="34" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1147,14 +1201,14 @@
       <c r="I34">
         <v>1</v>
       </c>
-      <c r="T34">
-        <v>1</v>
-      </c>
-      <c r="U34" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="AD34">
+        <v>1</v>
+      </c>
+      <c r="AE34" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="35" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1167,14 +1221,14 @@
       <c r="I35">
         <v>2</v>
       </c>
-      <c r="T35">
-        <v>1</v>
-      </c>
-      <c r="U35" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="AD35">
+        <v>1</v>
+      </c>
+      <c r="AE35" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="36" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1187,14 +1241,14 @@
       <c r="I36">
         <v>0</v>
       </c>
-      <c r="T36">
-        <v>1</v>
-      </c>
-      <c r="U36" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="AD36">
+        <v>1</v>
+      </c>
+      <c r="AE36" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="37" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1207,14 +1261,14 @@
       <c r="I37">
         <v>1</v>
       </c>
-      <c r="T37">
-        <v>1</v>
-      </c>
-      <c r="U37" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="AD37">
+        <v>1</v>
+      </c>
+      <c r="AE37" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="38" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1227,14 +1281,14 @@
       <c r="I38">
         <v>2</v>
       </c>
-      <c r="T38">
-        <v>1</v>
-      </c>
-      <c r="U38" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="AD38">
+        <v>1</v>
+      </c>
+      <c r="AE38" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="39" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1247,14 +1301,14 @@
       <c r="I39">
         <v>0</v>
       </c>
-      <c r="T39">
-        <v>1</v>
-      </c>
-      <c r="U39" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="AD39">
+        <v>1</v>
+      </c>
+      <c r="AE39" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="40" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1267,14 +1321,14 @@
       <c r="I40">
         <v>1</v>
       </c>
-      <c r="T40">
-        <v>1</v>
-      </c>
-      <c r="U40" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="AD40">
+        <v>1</v>
+      </c>
+      <c r="AE40" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="41" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1287,11 +1341,343 @@
       <c r="I41">
         <v>2</v>
       </c>
-      <c r="T41">
-        <v>1</v>
-      </c>
-      <c r="U41" t="s">
-        <v>41</v>
+      <c r="AD41">
+        <v>1</v>
+      </c>
+      <c r="AE41" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="42" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="J42">
+        <v>0</v>
+      </c>
+      <c r="K42">
+        <v>0</v>
+      </c>
+      <c r="L42">
+        <v>1</v>
+      </c>
+      <c r="M42">
+        <v>1</v>
+      </c>
+      <c r="N42">
+        <v>0</v>
+      </c>
+      <c r="AC42">
+        <v>1</v>
+      </c>
+      <c r="AE42" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="43" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="J43">
+        <v>0</v>
+      </c>
+      <c r="K43">
+        <v>0</v>
+      </c>
+      <c r="L43">
+        <v>1</v>
+      </c>
+      <c r="M43">
+        <v>1</v>
+      </c>
+      <c r="N43">
+        <v>2</v>
+      </c>
+      <c r="AE43" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="44" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="J44">
+        <v>0</v>
+      </c>
+      <c r="K44">
+        <v>2</v>
+      </c>
+      <c r="L44">
+        <v>1</v>
+      </c>
+      <c r="M44">
+        <v>1</v>
+      </c>
+      <c r="N44">
+        <v>0</v>
+      </c>
+      <c r="AE44" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="J45">
+        <v>0</v>
+      </c>
+      <c r="K45">
+        <v>2</v>
+      </c>
+      <c r="L45">
+        <v>1</v>
+      </c>
+      <c r="M45">
+        <v>1</v>
+      </c>
+      <c r="N45">
+        <v>2</v>
+      </c>
+      <c r="AE45" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="46" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="J46">
+        <v>2</v>
+      </c>
+      <c r="K46">
+        <v>0</v>
+      </c>
+      <c r="L46">
+        <v>1</v>
+      </c>
+      <c r="M46">
+        <v>1</v>
+      </c>
+      <c r="N46">
+        <v>0</v>
+      </c>
+      <c r="AC46">
+        <v>1</v>
+      </c>
+      <c r="AE46" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="47" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="J47">
+        <v>2</v>
+      </c>
+      <c r="K47">
+        <v>0</v>
+      </c>
+      <c r="L47">
+        <v>1</v>
+      </c>
+      <c r="M47">
+        <v>1</v>
+      </c>
+      <c r="N47">
+        <v>2</v>
+      </c>
+      <c r="AE47" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="48" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="J48">
+        <v>2</v>
+      </c>
+      <c r="K48">
+        <v>2</v>
+      </c>
+      <c r="L48">
+        <v>1</v>
+      </c>
+      <c r="M48">
+        <v>1</v>
+      </c>
+      <c r="N48">
+        <v>0</v>
+      </c>
+      <c r="AE48" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="49" spans="10:31" x14ac:dyDescent="0.2">
+      <c r="J49">
+        <v>2</v>
+      </c>
+      <c r="K49">
+        <v>2</v>
+      </c>
+      <c r="L49">
+        <v>1</v>
+      </c>
+      <c r="M49">
+        <v>1</v>
+      </c>
+      <c r="N49">
+        <v>2</v>
+      </c>
+      <c r="AE49" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="50" spans="10:31" x14ac:dyDescent="0.2">
+      <c r="O50" s="1">
+        <v>0</v>
+      </c>
+      <c r="P50" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q50" s="1">
+        <v>1</v>
+      </c>
+      <c r="R50" s="1">
+        <v>1</v>
+      </c>
+      <c r="S50" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD50">
+        <v>1</v>
+      </c>
+      <c r="AE50" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="51" spans="10:31" x14ac:dyDescent="0.2">
+      <c r="O51" s="1">
+        <v>0</v>
+      </c>
+      <c r="P51" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q51" s="1">
+        <v>1</v>
+      </c>
+      <c r="R51" s="1">
+        <v>1</v>
+      </c>
+      <c r="S51" s="1">
+        <v>2</v>
+      </c>
+      <c r="AE51" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="52" spans="10:31" x14ac:dyDescent="0.2">
+      <c r="O52" s="1">
+        <v>0</v>
+      </c>
+      <c r="P52" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q52" s="1">
+        <v>1</v>
+      </c>
+      <c r="R52" s="1">
+        <v>1</v>
+      </c>
+      <c r="S52" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE52" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="53" spans="10:31" x14ac:dyDescent="0.2">
+      <c r="O53" s="1">
+        <v>0</v>
+      </c>
+      <c r="P53" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q53" s="1">
+        <v>1</v>
+      </c>
+      <c r="R53" s="1">
+        <v>1</v>
+      </c>
+      <c r="S53" s="1">
+        <v>2</v>
+      </c>
+      <c r="AE53" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="54" spans="10:31" x14ac:dyDescent="0.2">
+      <c r="O54" s="1">
+        <v>2</v>
+      </c>
+      <c r="P54" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q54" s="1">
+        <v>1</v>
+      </c>
+      <c r="R54" s="1">
+        <v>1</v>
+      </c>
+      <c r="S54" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD54">
+        <v>1</v>
+      </c>
+      <c r="AE54" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="55" spans="10:31" x14ac:dyDescent="0.2">
+      <c r="O55" s="1">
+        <v>2</v>
+      </c>
+      <c r="P55" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q55" s="1">
+        <v>1</v>
+      </c>
+      <c r="R55" s="1">
+        <v>1</v>
+      </c>
+      <c r="S55" s="1">
+        <v>2</v>
+      </c>
+      <c r="AE55" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="56" spans="10:31" x14ac:dyDescent="0.2">
+      <c r="O56" s="1">
+        <v>2</v>
+      </c>
+      <c r="P56" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q56" s="1">
+        <v>1</v>
+      </c>
+      <c r="R56" s="1">
+        <v>1</v>
+      </c>
+      <c r="S56" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE56" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="57" spans="10:31" x14ac:dyDescent="0.2">
+      <c r="O57" s="1">
+        <v>2</v>
+      </c>
+      <c r="P57" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q57" s="1">
+        <v>1</v>
+      </c>
+      <c r="R57" s="1">
+        <v>1</v>
+      </c>
+      <c r="S57" s="1">
+        <v>2</v>
+      </c>
+      <c r="AE57" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>